<commit_message>
feat: attribute for route
</commit_message>
<xml_diff>
--- a/scripts/excel/route.xlsx
+++ b/scripts/excel/route.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Program Files\File Tugas Sekolah\Kelas 12\Semester 1\PKK\(1) Tugas Produksi Massal\api-center\scripts\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7801E544-E5D3-43FA-AC1E-DEA0FF76C3F1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CB83A38-4E66-4F63-B022-5210EA31E20A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3852" yWindow="3144" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="38">
   <si>
     <t>No.</t>
   </si>
@@ -105,16 +105,40 @@
     <t>Amount - Determines the amount of data</t>
   </si>
   <si>
-    <t>random/student/smk/amount/{amount}</t>
-  </si>
-  <si>
-    <t>random/student/sma/amount/{amount}</t>
-  </si>
-  <si>
     <t>random/student/smk/amount/10</t>
   </si>
   <si>
     <t>random/student/sma/amount/10</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>Id, Name</t>
+  </si>
+  <si>
+    <t>Id, Birth Place</t>
+  </si>
+  <si>
+    <t>Id, Religion</t>
+  </si>
+  <si>
+    <t>Id, SMK Major</t>
+  </si>
+  <si>
+    <t>Id, SMA Major</t>
+  </si>
+  <si>
+    <t>Id, Type, Value</t>
+  </si>
+  <si>
+    <t>Id, NIS, Name, Age, Birth Place, Birth Date, Gender, Grade, Major</t>
+  </si>
+  <si>
+    <t>random/student/smk/amount/:amount</t>
+  </si>
+  <si>
+    <t>random/student/sma/amount/:amount</t>
   </si>
 </sst>
 </file>
@@ -173,7 +197,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -184,6 +208,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="D4:H15"/>
+  <dimension ref="D4:I15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -477,9 +505,10 @@
     <col min="6" max="6" width="28.6640625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="35.21875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="48.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="54" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="4:8" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="4:9" ht="15.6" x14ac:dyDescent="0.3">
       <c r="D4" s="3" t="s">
         <v>0</v>
       </c>
@@ -495,8 +524,11 @@
       <c r="H4" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="I4" s="4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D5" s="1">
         <v>1</v>
       </c>
@@ -510,8 +542,11 @@
       <c r="H5" s="2" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="6" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="I5" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D6" s="1">
         <v>2</v>
       </c>
@@ -525,8 +560,11 @@
       <c r="H6" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="7" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="I6" s="5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D7" s="1">
         <v>3</v>
       </c>
@@ -540,8 +578,11 @@
       <c r="H7" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="8" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="I7" s="5" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D8" s="1">
         <v>4</v>
       </c>
@@ -555,8 +596,11 @@
       <c r="H8" s="2" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="9" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="I8" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D9" s="1">
         <v>5</v>
       </c>
@@ -570,8 +614,11 @@
       <c r="H9" s="2" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="10" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="I9" s="5" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D10" s="1">
         <v>6</v>
       </c>
@@ -585,8 +632,11 @@
       <c r="H10" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="11" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="I10" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D11" s="1">
         <v>7</v>
       </c>
@@ -600,8 +650,11 @@
       <c r="H11" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="12" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="I11" s="5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D12" s="1">
         <v>8</v>
       </c>
@@ -615,16 +668,19 @@
       <c r="H12" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="13" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="I12" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D13" s="1">
         <v>9</v>
       </c>
       <c r="E13" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>26</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>28</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>25</v>
@@ -632,8 +688,11 @@
       <c r="H13" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="14" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="I13" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D14" s="1">
         <v>10</v>
       </c>
@@ -647,22 +706,28 @@
       <c r="H14" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="15" spans="4:8" x14ac:dyDescent="0.3">
+      <c r="I14" s="5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="4:9" x14ac:dyDescent="0.3">
       <c r="D15" s="1">
         <v>11</v>
       </c>
       <c r="E15" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>25</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="I15" s="5" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>